<commit_message>
Changed terrain type to habitat
</commit_message>
<xml_diff>
--- a/datasets/JJ_DATA.xlsx
+++ b/datasets/JJ_DATA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jj/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jj/Local Documents/Ben's Research/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AB29AE3B-7019-3240-BBD1-61F7B57A10A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905C13AA-E090-3341-8FFA-9F87C6764E6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{E59EF2F2-ACB7-478F-A728-D3B8442404FE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" xr2:uid="{E59EF2F2-ACB7-478F-A728-D3B8442404FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="58">
   <si>
     <t>Species</t>
-  </si>
-  <si>
-    <t>Terrain Type</t>
   </si>
   <si>
     <t>Hannidae sp 1.0</t>
@@ -210,6 +207,9 @@
   </si>
   <si>
     <t>West Beach West</t>
+  </si>
+  <si>
+    <t>Habitat</t>
   </si>
 </sst>
 </file>
@@ -599,7 +599,7 @@
   <dimension ref="A3:W191"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F130" sqref="F130"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -614,78 +614,78 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
         <v>34</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>35</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>36</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>37</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>38</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>39</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>40</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>41</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>42</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>43</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>44</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>45</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>46</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>47</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>48</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>49</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>50</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>51</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>52</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>53</v>
-      </c>
-      <c r="W3" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
         <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -748,15 +748,15 @@
         <v>0</v>
       </c>
       <c r="W5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -819,15 +819,15 @@
         <v>0</v>
       </c>
       <c r="W6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -890,15 +890,15 @@
         <v>0</v>
       </c>
       <c r="W7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -961,15 +961,15 @@
         <v>0</v>
       </c>
       <c r="W8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1032,15 +1032,15 @@
         <v>0</v>
       </c>
       <c r="W9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1103,15 +1103,15 @@
         <v>0</v>
       </c>
       <c r="W10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1174,15 +1174,15 @@
         <v>0</v>
       </c>
       <c r="W11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1245,15 +1245,15 @@
         <v>0</v>
       </c>
       <c r="W12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1316,15 +1316,15 @@
         <v>0</v>
       </c>
       <c r="W13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1387,15 +1387,15 @@
         <v>0</v>
       </c>
       <c r="W14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1458,15 +1458,15 @@
         <v>0</v>
       </c>
       <c r="W15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1529,15 +1529,15 @@
         <v>0</v>
       </c>
       <c r="W16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1600,15 +1600,15 @@
         <v>0</v>
       </c>
       <c r="W17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1671,15 +1671,15 @@
         <v>0</v>
       </c>
       <c r="W18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1742,15 +1742,15 @@
         <v>0</v>
       </c>
       <c r="W19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -1813,15 +1813,15 @@
         <v>0</v>
       </c>
       <c r="W20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -1884,15 +1884,15 @@
         <v>0</v>
       </c>
       <c r="W21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -1955,15 +1955,15 @@
         <v>0</v>
       </c>
       <c r="W22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B23" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -2026,15 +2026,15 @@
         <v>0</v>
       </c>
       <c r="W23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -2097,15 +2097,15 @@
         <v>0</v>
       </c>
       <c r="W24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B25" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -2168,15 +2168,15 @@
         <v>0</v>
       </c>
       <c r="W25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B26" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -2239,15 +2239,15 @@
         <v>0</v>
       </c>
       <c r="W26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B27" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -2310,15 +2310,15 @@
         <v>0</v>
       </c>
       <c r="W27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B28" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -2381,15 +2381,15 @@
         <v>0</v>
       </c>
       <c r="W28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B29" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -2452,15 +2452,15 @@
         <v>0</v>
       </c>
       <c r="W29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -2523,15 +2523,15 @@
         <v>0</v>
       </c>
       <c r="W30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B31" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -2594,15 +2594,15 @@
         <v>0</v>
       </c>
       <c r="W31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B32" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -2665,15 +2665,15 @@
         <v>0</v>
       </c>
       <c r="W32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B33" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -2736,15 +2736,15 @@
         <v>0</v>
       </c>
       <c r="W33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B34" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -2807,15 +2807,15 @@
         <v>0</v>
       </c>
       <c r="W34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B35" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -2878,15 +2878,15 @@
         <v>0</v>
       </c>
       <c r="W35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B36" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -2949,15 +2949,15 @@
         <v>0</v>
       </c>
       <c r="W36" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B37" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -3020,15 +3020,15 @@
         <v>0</v>
       </c>
       <c r="W37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B38" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -3091,15 +3091,15 @@
         <v>0</v>
       </c>
       <c r="W38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B39" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -3162,15 +3162,15 @@
         <v>0</v>
       </c>
       <c r="W39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B40" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -3233,15 +3233,15 @@
         <v>0</v>
       </c>
       <c r="W40" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B41" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -3304,15 +3304,15 @@
         <v>0</v>
       </c>
       <c r="W41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B42" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -3375,15 +3375,15 @@
         <v>0</v>
       </c>
       <c r="W42" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B43" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -3446,15 +3446,15 @@
         <v>0</v>
       </c>
       <c r="W43" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B44" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C44">
         <v>2</v>
@@ -3517,15 +3517,15 @@
         <v>0</v>
       </c>
       <c r="W44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B45" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C45">
         <v>0</v>
@@ -3588,15 +3588,15 @@
         <v>0</v>
       </c>
       <c r="W45" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B46" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -3659,15 +3659,15 @@
         <v>0</v>
       </c>
       <c r="W46" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B47" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -3730,15 +3730,15 @@
         <v>0</v>
       </c>
       <c r="W47" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B48" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -3801,15 +3801,15 @@
         <v>0</v>
       </c>
       <c r="W48" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B49" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -3872,15 +3872,15 @@
         <v>0</v>
       </c>
       <c r="W49" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="50" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B50" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -3943,15 +3943,15 @@
         <v>0</v>
       </c>
       <c r="W50" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B51" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -4014,15 +4014,15 @@
         <v>0</v>
       </c>
       <c r="W51" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="52" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B52" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -4085,15 +4085,15 @@
         <v>0</v>
       </c>
       <c r="W52" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B53" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -4156,15 +4156,15 @@
         <v>0</v>
       </c>
       <c r="W53" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B54" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C54">
         <v>0</v>
@@ -4227,15 +4227,15 @@
         <v>0</v>
       </c>
       <c r="W54" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B55" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C55">
         <v>0</v>
@@ -4298,15 +4298,15 @@
         <v>0</v>
       </c>
       <c r="W55" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B56" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C56">
         <v>0</v>
@@ -4369,15 +4369,15 @@
         <v>0</v>
       </c>
       <c r="W56" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B57" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -4440,15 +4440,15 @@
         <v>0</v>
       </c>
       <c r="W57" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="58" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B58" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -4511,15 +4511,15 @@
         <v>0</v>
       </c>
       <c r="W58" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="59" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B59" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -4582,15 +4582,15 @@
         <v>0</v>
       </c>
       <c r="W59" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="60" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B60" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C60">
         <v>0</v>
@@ -4653,15 +4653,15 @@
         <v>0</v>
       </c>
       <c r="W60" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="61" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B61" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -4724,15 +4724,15 @@
         <v>0</v>
       </c>
       <c r="W61" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="62" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B62" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -4795,15 +4795,15 @@
         <v>0</v>
       </c>
       <c r="W62" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="63" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B63" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -4866,15 +4866,15 @@
         <v>0</v>
       </c>
       <c r="W63" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="64" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B64" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -4937,16 +4937,16 @@
         <v>0</v>
       </c>
       <c r="W64" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="69" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
+        <v>1</v>
+      </c>
+      <c r="B69" t="s">
         <v>2</v>
       </c>
-      <c r="B69" t="s">
-        <v>3</v>
-      </c>
       <c r="C69">
         <v>0</v>
       </c>
@@ -5008,15 +5008,15 @@
         <v>0</v>
       </c>
       <c r="W69" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="70" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B70" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C70">
         <v>0</v>
@@ -5079,15 +5079,15 @@
         <v>0</v>
       </c>
       <c r="W70" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="71" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B71" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C71">
         <v>0</v>
@@ -5150,15 +5150,15 @@
         <v>0</v>
       </c>
       <c r="W71" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="72" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B72" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C72">
         <v>0</v>
@@ -5221,15 +5221,15 @@
         <v>0</v>
       </c>
       <c r="W72" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="73" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B73" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C73">
         <v>0</v>
@@ -5292,15 +5292,15 @@
         <v>0</v>
       </c>
       <c r="W73" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="74" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B74" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C74">
         <v>0</v>
@@ -5363,15 +5363,15 @@
         <v>0</v>
       </c>
       <c r="W74" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="75" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B75" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C75">
         <v>0</v>
@@ -5434,15 +5434,15 @@
         <v>0</v>
       </c>
       <c r="W75" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="76" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B76" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C76">
         <v>0</v>
@@ -5505,15 +5505,15 @@
         <v>0</v>
       </c>
       <c r="W76" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="77" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B77" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C77">
         <v>0</v>
@@ -5576,15 +5576,15 @@
         <v>0</v>
       </c>
       <c r="W77" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="78" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B78" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C78">
         <v>0</v>
@@ -5647,15 +5647,15 @@
         <v>0</v>
       </c>
       <c r="W78" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="79" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B79" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C79">
         <v>0</v>
@@ -5718,15 +5718,15 @@
         <v>0</v>
       </c>
       <c r="W79" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="80" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B80" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C80">
         <v>0</v>
@@ -5789,15 +5789,15 @@
         <v>0</v>
       </c>
       <c r="W80" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="81" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B81" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C81">
         <v>0</v>
@@ -5860,15 +5860,15 @@
         <v>0</v>
       </c>
       <c r="W81" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="82" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B82" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C82">
         <v>0</v>
@@ -5931,15 +5931,15 @@
         <v>0</v>
       </c>
       <c r="W82" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="83" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B83" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C83">
         <v>0</v>
@@ -6002,15 +6002,15 @@
         <v>0</v>
       </c>
       <c r="W83" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="84" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B84" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C84">
         <v>0</v>
@@ -6073,15 +6073,15 @@
         <v>0</v>
       </c>
       <c r="W84" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="85" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B85" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C85">
         <v>0</v>
@@ -6144,15 +6144,15 @@
         <v>0</v>
       </c>
       <c r="W85" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="86" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B86" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C86">
         <v>0</v>
@@ -6215,15 +6215,15 @@
         <v>0</v>
       </c>
       <c r="W86" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="87" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B87" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C87">
         <v>0</v>
@@ -6286,15 +6286,15 @@
         <v>0</v>
       </c>
       <c r="W87" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="88" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B88" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C88">
         <v>0</v>
@@ -6357,15 +6357,15 @@
         <v>0</v>
       </c>
       <c r="W88" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="89" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B89" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C89">
         <v>0</v>
@@ -6428,15 +6428,15 @@
         <v>0</v>
       </c>
       <c r="W89" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="90" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B90" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C90">
         <v>0</v>
@@ -6499,15 +6499,15 @@
         <v>0</v>
       </c>
       <c r="W90" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="91" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B91" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C91">
         <v>0</v>
@@ -6570,15 +6570,15 @@
         <v>0</v>
       </c>
       <c r="W91" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="92" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B92" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C92">
         <v>0</v>
@@ -6641,15 +6641,15 @@
         <v>0</v>
       </c>
       <c r="W92" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="93" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B93" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C93">
         <v>0</v>
@@ -6712,15 +6712,15 @@
         <v>0</v>
       </c>
       <c r="W93" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="94" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B94" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C94">
         <v>0</v>
@@ -6783,15 +6783,15 @@
         <v>0</v>
       </c>
       <c r="W94" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="95" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B95" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C95">
         <v>0</v>
@@ -6854,15 +6854,15 @@
         <v>0</v>
       </c>
       <c r="W95" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="96" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B96" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C96">
         <v>0</v>
@@ -6925,15 +6925,15 @@
         <v>0</v>
       </c>
       <c r="W96" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="97" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B97" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C97">
         <v>0</v>
@@ -6996,15 +6996,15 @@
         <v>0</v>
       </c>
       <c r="W97" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="98" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B98" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C98">
         <v>0</v>
@@ -7067,15 +7067,15 @@
         <v>0</v>
       </c>
       <c r="W98" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="99" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B99" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C99">
         <v>0</v>
@@ -7138,15 +7138,15 @@
         <v>0</v>
       </c>
       <c r="W99" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="100" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B100" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C100">
         <v>0</v>
@@ -7209,15 +7209,15 @@
         <v>0</v>
       </c>
       <c r="W100" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="101" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B101" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C101">
         <v>0</v>
@@ -7280,15 +7280,15 @@
         <v>0</v>
       </c>
       <c r="W101" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="102" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B102" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C102">
         <v>0</v>
@@ -7351,15 +7351,15 @@
         <v>0</v>
       </c>
       <c r="W102" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="103" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B103" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C103">
         <v>0</v>
@@ -7422,15 +7422,15 @@
         <v>0</v>
       </c>
       <c r="W103" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="104" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B104" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C104">
         <v>0</v>
@@ -7493,15 +7493,15 @@
         <v>0</v>
       </c>
       <c r="W104" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="105" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B105" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C105">
         <v>0</v>
@@ -7564,15 +7564,15 @@
         <v>0</v>
       </c>
       <c r="W105" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="106" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B106" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C106">
         <v>0</v>
@@ -7635,15 +7635,15 @@
         <v>0</v>
       </c>
       <c r="W106" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="107" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B107" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C107">
         <v>0</v>
@@ -7706,15 +7706,15 @@
         <v>0</v>
       </c>
       <c r="W107" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="108" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B108" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C108">
         <v>0</v>
@@ -7777,15 +7777,15 @@
         <v>0</v>
       </c>
       <c r="W108" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="109" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B109" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C109">
         <v>0</v>
@@ -7848,15 +7848,15 @@
         <v>0</v>
       </c>
       <c r="W109" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="110" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B110" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C110">
         <v>0</v>
@@ -7919,15 +7919,15 @@
         <v>0</v>
       </c>
       <c r="W110" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="111" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B111" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C111">
         <v>0</v>
@@ -7990,15 +7990,15 @@
         <v>0</v>
       </c>
       <c r="W111" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="112" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B112" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C112">
         <v>0</v>
@@ -8061,15 +8061,15 @@
         <v>0</v>
       </c>
       <c r="W112" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="113" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B113" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C113">
         <v>0</v>
@@ -8132,15 +8132,15 @@
         <v>0</v>
       </c>
       <c r="W113" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="114" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B114" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C114">
         <v>0</v>
@@ -8203,15 +8203,15 @@
         <v>0</v>
       </c>
       <c r="W114" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="115" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B115" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C115">
         <v>5</v>
@@ -8274,15 +8274,15 @@
         <v>0</v>
       </c>
       <c r="W115" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="116" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B116" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C116">
         <v>0</v>
@@ -8345,15 +8345,15 @@
         <v>0</v>
       </c>
       <c r="W116" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="117" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B117" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C117">
         <v>0</v>
@@ -8416,15 +8416,15 @@
         <v>0</v>
       </c>
       <c r="W117" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="118" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B118" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C118">
         <v>0</v>
@@ -8487,15 +8487,15 @@
         <v>2</v>
       </c>
       <c r="W118" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="119" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B119" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C119">
         <v>1</v>
@@ -8558,15 +8558,15 @@
         <v>0</v>
       </c>
       <c r="W119" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="120" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B120" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C120">
         <v>0</v>
@@ -8629,15 +8629,15 @@
         <v>0</v>
       </c>
       <c r="W120" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="121" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B121" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C121">
         <v>0</v>
@@ -8700,15 +8700,15 @@
         <v>0</v>
       </c>
       <c r="W121" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="122" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B122" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C122">
         <v>0</v>
@@ -8771,15 +8771,15 @@
         <v>0</v>
       </c>
       <c r="W122" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="123" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B123" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C123">
         <v>0</v>
@@ -8842,15 +8842,15 @@
         <v>0</v>
       </c>
       <c r="W123" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="124" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B124" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C124">
         <v>0</v>
@@ -8913,15 +8913,15 @@
         <v>0</v>
       </c>
       <c r="W124" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="125" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B125" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C125">
         <v>0</v>
@@ -8984,15 +8984,15 @@
         <v>0</v>
       </c>
       <c r="W125" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="126" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B126" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C126">
         <v>0</v>
@@ -9055,15 +9055,15 @@
         <v>0</v>
       </c>
       <c r="W126" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="127" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B127" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C127">
         <v>0</v>
@@ -9126,15 +9126,15 @@
         <v>0</v>
       </c>
       <c r="W127" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="128" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B128" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C128">
         <v>0</v>
@@ -9197,15 +9197,15 @@
         <v>0</v>
       </c>
       <c r="W128" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="132" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
+        <v>1</v>
+      </c>
+      <c r="B132" t="s">
         <v>2</v>
-      </c>
-      <c r="B132" t="s">
-        <v>3</v>
       </c>
       <c r="C132">
         <v>0</v>
@@ -9268,15 +9268,15 @@
         <v>0</v>
       </c>
       <c r="W132" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="133" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B133" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C133">
         <v>0</v>
@@ -9339,15 +9339,15 @@
         <v>0</v>
       </c>
       <c r="W133" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="134" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B134" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C134">
         <v>0</v>
@@ -9410,15 +9410,15 @@
         <v>0</v>
       </c>
       <c r="W134" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="135" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B135" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C135">
         <v>0</v>
@@ -9481,15 +9481,15 @@
         <v>0</v>
       </c>
       <c r="W135" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="136" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B136" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C136">
         <v>0</v>
@@ -9552,15 +9552,15 @@
         <v>0</v>
       </c>
       <c r="W136" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="137" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B137" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C137">
         <v>0</v>
@@ -9623,15 +9623,15 @@
         <v>0</v>
       </c>
       <c r="W137" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="138" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B138" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C138">
         <v>0</v>
@@ -9694,15 +9694,15 @@
         <v>0</v>
       </c>
       <c r="W138" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="139" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B139" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C139">
         <v>0</v>
@@ -9765,15 +9765,15 @@
         <v>0</v>
       </c>
       <c r="W139" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="140" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B140" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C140">
         <v>0</v>
@@ -9836,15 +9836,15 @@
         <v>0</v>
       </c>
       <c r="W140" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="141" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B141" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C141">
         <v>0</v>
@@ -9907,15 +9907,15 @@
         <v>0</v>
       </c>
       <c r="W141" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="142" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B142" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C142">
         <v>0</v>
@@ -9978,15 +9978,15 @@
         <v>0</v>
       </c>
       <c r="W142" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="143" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B143" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C143">
         <v>0</v>
@@ -10049,15 +10049,15 @@
         <v>0</v>
       </c>
       <c r="W143" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="144" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B144" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C144">
         <v>0</v>
@@ -10120,15 +10120,15 @@
         <v>0</v>
       </c>
       <c r="W144" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="145" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B145" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C145">
         <v>0</v>
@@ -10191,15 +10191,15 @@
         <v>0</v>
       </c>
       <c r="W145" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="146" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B146" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C146">
         <v>0</v>
@@ -10262,15 +10262,15 @@
         <v>0</v>
       </c>
       <c r="W146" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="147" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B147" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C147">
         <v>0</v>
@@ -10333,15 +10333,15 @@
         <v>0</v>
       </c>
       <c r="W147" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="148" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B148" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C148">
         <v>0</v>
@@ -10404,15 +10404,15 @@
         <v>0</v>
       </c>
       <c r="W148" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="149" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B149" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C149">
         <v>0</v>
@@ -10475,15 +10475,15 @@
         <v>0</v>
       </c>
       <c r="W149" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="150" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B150" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C150">
         <v>0</v>
@@ -10546,15 +10546,15 @@
         <v>0</v>
       </c>
       <c r="W150" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="151" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B151" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C151">
         <v>0</v>
@@ -10617,15 +10617,15 @@
         <v>0</v>
       </c>
       <c r="W151" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="152" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B152" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C152">
         <v>0</v>
@@ -10688,15 +10688,15 @@
         <v>0</v>
       </c>
       <c r="W152" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="153" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B153" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C153">
         <v>0</v>
@@ -10759,15 +10759,15 @@
         <v>0</v>
       </c>
       <c r="W153" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="154" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B154" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C154">
         <v>0</v>
@@ -10830,15 +10830,15 @@
         <v>0</v>
       </c>
       <c r="W154" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="155" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B155" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C155">
         <v>0</v>
@@ -10901,15 +10901,15 @@
         <v>0</v>
       </c>
       <c r="W155" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="156" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B156" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C156">
         <v>0</v>
@@ -10972,15 +10972,15 @@
         <v>0</v>
       </c>
       <c r="W156" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="157" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B157" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C157">
         <v>0</v>
@@ -11043,15 +11043,15 @@
         <v>0</v>
       </c>
       <c r="W157" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="158" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B158" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C158">
         <v>0</v>
@@ -11114,15 +11114,15 @@
         <v>0</v>
       </c>
       <c r="W158" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="159" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B159" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C159">
         <v>0</v>
@@ -11185,15 +11185,15 @@
         <v>0</v>
       </c>
       <c r="W159" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="160" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B160" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C160">
         <v>0</v>
@@ -11256,15 +11256,15 @@
         <v>0</v>
       </c>
       <c r="W160" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="161" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B161" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C161">
         <v>0</v>
@@ -11327,15 +11327,15 @@
         <v>0</v>
       </c>
       <c r="W161" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="162" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B162" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C162">
         <v>0</v>
@@ -11398,15 +11398,15 @@
         <v>0</v>
       </c>
       <c r="W162" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="163" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B163" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C163">
         <v>0</v>
@@ -11469,15 +11469,15 @@
         <v>0</v>
       </c>
       <c r="W163" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="164" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B164" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C164">
         <v>0</v>
@@ -11540,15 +11540,15 @@
         <v>0</v>
       </c>
       <c r="W164" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="165" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B165" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C165">
         <v>0</v>
@@ -11611,15 +11611,15 @@
         <v>0</v>
       </c>
       <c r="W165" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="166" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B166" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C166">
         <v>0</v>
@@ -11682,15 +11682,15 @@
         <v>0</v>
       </c>
       <c r="W166" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="167" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B167" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C167">
         <v>0</v>
@@ -11753,15 +11753,15 @@
         <v>0</v>
       </c>
       <c r="W167" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="168" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B168" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C168">
         <v>0</v>
@@ -11824,15 +11824,15 @@
         <v>0</v>
       </c>
       <c r="W168" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="169" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B169" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C169">
         <v>0</v>
@@ -11895,15 +11895,15 @@
         <v>0</v>
       </c>
       <c r="W169" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="170" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B170" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C170">
         <v>0</v>
@@ -11966,15 +11966,15 @@
         <v>0</v>
       </c>
       <c r="W170" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="171" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B171" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C171">
         <v>0</v>
@@ -12037,15 +12037,15 @@
         <v>0</v>
       </c>
       <c r="W171" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="172" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B172" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C172">
         <v>0</v>
@@ -12108,15 +12108,15 @@
         <v>0</v>
       </c>
       <c r="W172" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="173" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B173" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C173">
         <v>0</v>
@@ -12179,15 +12179,15 @@
         <v>0</v>
       </c>
       <c r="W173" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="174" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B174" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C174">
         <v>0</v>
@@ -12250,15 +12250,15 @@
         <v>0</v>
       </c>
       <c r="W174" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="175" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B175" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C175">
         <v>0</v>
@@ -12321,15 +12321,15 @@
         <v>0</v>
       </c>
       <c r="W175" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="176" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B176" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C176">
         <v>0</v>
@@ -12392,15 +12392,15 @@
         <v>0</v>
       </c>
       <c r="W176" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="177" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B177" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C177">
         <v>0</v>
@@ -12463,15 +12463,15 @@
         <v>0</v>
       </c>
       <c r="W177" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="178" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B178" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C178">
         <v>0</v>
@@ -12534,15 +12534,15 @@
         <v>0</v>
       </c>
       <c r="W178" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="179" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B179" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C179">
         <v>0</v>
@@ -12605,15 +12605,15 @@
         <v>0</v>
       </c>
       <c r="W179" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="180" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B180" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C180">
         <v>0</v>
@@ -12676,15 +12676,15 @@
         <v>0</v>
       </c>
       <c r="W180" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="181" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B181" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C181">
         <v>0</v>
@@ -12747,15 +12747,15 @@
         <v>2</v>
       </c>
       <c r="W181" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="182" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B182" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C182">
         <v>0</v>
@@ -12818,15 +12818,15 @@
         <v>0</v>
       </c>
       <c r="W182" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="183" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B183" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C183">
         <v>0</v>
@@ -12889,15 +12889,15 @@
         <v>0</v>
       </c>
       <c r="W183" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="184" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B184" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C184">
         <v>0</v>
@@ -12960,15 +12960,15 @@
         <v>0</v>
       </c>
       <c r="W184" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="185" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B185" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C185">
         <v>0</v>
@@ -13031,15 +13031,15 @@
         <v>0</v>
       </c>
       <c r="W185" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="186" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B186" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C186">
         <v>0</v>
@@ -13102,15 +13102,15 @@
         <v>0</v>
       </c>
       <c r="W186" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="187" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B187" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C187">
         <v>0</v>
@@ -13173,15 +13173,15 @@
         <v>0</v>
       </c>
       <c r="W187" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="188" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B188" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C188">
         <v>0</v>
@@ -13244,15 +13244,15 @@
         <v>0</v>
       </c>
       <c r="W188" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="189" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B189" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C189">
         <v>0</v>
@@ -13315,15 +13315,15 @@
         <v>0</v>
       </c>
       <c r="W189" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="190" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B190" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C190">
         <v>0</v>
@@ -13386,15 +13386,15 @@
         <v>0</v>
       </c>
       <c r="W190" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="191" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B191" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C191">
         <v>0</v>
@@ -13457,7 +13457,7 @@
         <v>0</v>
       </c>
       <c r="W191" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>